<commit_message>
Símbolos de € y % en resultados
</commit_message>
<xml_diff>
--- a/Simulación penalización IPF_deposito_creciente.xlsx
+++ b/Simulación penalización IPF_deposito_creciente.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u323394\OneDrive - Caja Rural de Navarra\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\OneDrive - sysadmit.com\GitRepos\CJ\Simulaciion penalizacion IPF - Deposito Creciente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="CRECIENTE 18M" sheetId="3" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="43">
   <si>
     <t>Importe</t>
   </si>
@@ -127,17 +128,38 @@
   </si>
   <si>
     <t>REINTEGRO DEPOSITO CRECIENTE 18M - Penalización por días transcurridos (Tarifas coyunturales)</t>
+  </si>
+  <si>
+    <t>Resultados</t>
+  </si>
+  <si>
+    <t>% Retención</t>
+  </si>
+  <si>
+    <t>Retención Euros</t>
+  </si>
+  <si>
+    <t>+Intereses</t>
+  </si>
+  <si>
+    <t>-Retención</t>
+  </si>
+  <si>
+    <t>+Capital</t>
+  </si>
+  <si>
+    <t>-Penalización</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,8 +182,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +222,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -244,12 +292,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -260,74 +374,128 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -612,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -633,27 +801,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19">
-        <v>100000</v>
+      <c r="B3" s="18">
+        <v>15000</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -661,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>45000</v>
+        <v>45112</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -669,77 +837,77 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>45550</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>45662</v>
+      </c>
+      <c r="D5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="42"/>
+      <c r="G5" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="42"/>
+      <c r="J5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="42"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.02</v>
+      <c r="B6" s="5">
+        <v>0.03</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <f>+B3-E25</f>
-        <v>99500</v>
+        <v>10000</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <f>+E6-H25</f>
-        <v>98800</v>
+        <v>5000</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="19">
         <f>+H6-K25</f>
-        <v>98000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
-        <v>0.19</v>
+      <c r="B7" s="6">
+        <v>0.2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f>B10</f>
-        <v>45184</v>
+        <v>45296</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f>B16</f>
-        <v>45366</v>
+        <v>45478</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <f>B22</f>
-        <v>45550</v>
+        <v>45662</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -748,50 +916,50 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="23">
         <f>+E7-B4</f>
         <v>184</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="23">
         <f>+H7-E7</f>
         <v>182</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="23">
         <f>+K7-H7</f>
         <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>B11</f>
-        <v>2.75E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <f>B17</f>
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <f>B23</f>
-        <v>3.7499999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -799,65 +967,65 @@
         <v>17</v>
       </c>
       <c r="B10" s="3">
-        <v>45184</v>
+        <v>45296</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <f>+E6*E9*E8/365</f>
-        <v>1379.3698630136987</v>
+        <v>100.82191780821918</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <f>+H6*H9*H8/365</f>
-        <v>1477.9397260273972</v>
+        <v>37.397260273972606</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="18">
         <f>+K6*K9*K8/365</f>
-        <v>1852.6027397260275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="6">
-        <v>2.75E-2</v>
+      <c r="B11" s="5">
+        <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="19">
-        <v>500</v>
+      <c r="B12" s="18">
+        <v>5000</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -865,28 +1033,28 @@
         <v>4</v>
       </c>
       <c r="B13" s="3">
-        <v>45061</v>
+        <v>45295</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <f>+E10*E12</f>
-        <v>262.08027397260275</v>
+        <v>20.164383561643838</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <f>+H10*H12</f>
-        <v>280.80854794520548</v>
+        <v>7.4794520547945211</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <f>+K10*K12</f>
-        <v>351.99452054794523</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -894,72 +1062,72 @@
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>45366</v>
-      </c>
-      <c r="D16" s="13" t="s">
+        <v>45478</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="G16" s="13" t="s">
+      <c r="E16" s="13"/>
+      <c r="G16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="J16" s="13" t="s">
+      <c r="H16" s="13"/>
+      <c r="J16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="14"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
+      <c r="B17" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19">
-        <v>700</v>
-      </c>
-      <c r="D18" s="15" t="s">
+      <c r="B18" s="18">
+        <v>5000</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <f>+E10</f>
-        <v>1379.3698630136987</v>
-      </c>
-      <c r="G18" s="15" t="s">
+        <v>100.82191780821918</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="20">
         <f>+H10</f>
-        <v>1477.9397260273972</v>
-      </c>
-      <c r="J18" s="15" t="s">
+        <v>37.397260273972606</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="20">
         <f>+K10</f>
-        <v>1852.6027397260275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -967,59 +1135,59 @@
         <v>4</v>
       </c>
       <c r="B19" s="3">
-        <v>45214</v>
-      </c>
-      <c r="D19" s="15" t="s">
+        <v>45478</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="20">
         <f>-E13</f>
-        <v>-262.08027397260275</v>
-      </c>
-      <c r="G19" s="15" t="s">
+        <v>-20.164383561643838</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="20">
         <f>-H13</f>
-        <v>-280.80854794520548</v>
-      </c>
-      <c r="J19" s="15" t="s">
+        <v>-7.4794520547945211</v>
+      </c>
+      <c r="J19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="20">
         <f>-K13</f>
-        <v>-351.99452054794523</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="22">
+      <c r="B21" s="9"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="21">
         <f>+SUM(E17:E20)</f>
-        <v>1117.289589041096</v>
-      </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="22">
+        <v>80.657534246575352</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="21">
         <f>+SUM(H17:H20)</f>
-        <v>1197.1311780821918</v>
-      </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="22">
+        <v>29.917808219178085</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="21">
         <f>+SUM(K17:K20)</f>
-        <v>1500.6082191780822</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1027,444 +1195,444 @@
         <v>17</v>
       </c>
       <c r="B22" s="3">
-        <v>45550</v>
+        <v>45662</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="6">
-        <v>3.7499999999999999E-2</v>
+      <c r="B23" s="5">
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="19">
-        <v>800</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="B24" s="18">
+        <v>5000</v>
+      </c>
+      <c r="D24" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="G24" s="4" t="s">
+      <c r="E24" s="42"/>
+      <c r="G24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="J24" s="4" t="s">
+      <c r="H24" s="42"/>
+      <c r="J24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="4"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="3">
-        <v>45397</v>
+        <v>45662</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="22">
         <f>B12</f>
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="22">
         <f>B18</f>
-        <v>700</v>
+        <v>5000</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="22">
         <f>B24</f>
-        <v>800</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
+      <c r="B26" s="8"/>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <f>B13</f>
-        <v>45061</v>
+        <v>45295</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <f>B19</f>
-        <v>45214</v>
+        <v>45478</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="7">
         <f>B25</f>
-        <v>45397</v>
+        <v>45662</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
+      <c r="B27" s="8"/>
       <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <f>$B$6</f>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="10">
         <f>$B$6</f>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="10">
         <f>$B$6</f>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
+      <c r="B28" s="8"/>
       <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="23">
         <f>+E26-B4</f>
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="23">
         <f>+H26-B4</f>
-        <v>214</v>
+        <v>366</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="24">
+      <c r="K28" s="23">
         <f>+K26-B4</f>
-        <v>397</v>
+        <v>550</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <f>+E28</f>
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="23">
         <f>+H26-E7</f>
-        <v>30</v>
+        <v>182</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="24">
+      <c r="K29" s="23">
         <f>+K26-H7</f>
-        <v>31</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="9"/>
+      <c r="B30" s="8"/>
       <c r="D30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <f>+E25*E9*E28/365</f>
-        <v>2.297945205479452</v>
+        <v>50.136986301369866</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="19">
         <f>+H25*H9*H29/365</f>
-        <v>1.726027397260274</v>
+        <v>37.397260273972606</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K30" s="19">
         <f>+K25*K9*K29/365</f>
-        <v>2.547945205479452</v>
+        <v>25.205479452054796</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="9"/>
+      <c r="B31" s="8"/>
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="19">
         <f>+E25*E28*E27/365</f>
-        <v>1.6712328767123288</v>
+        <v>75.205479452054789</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="20">
+      <c r="H31" s="19">
         <f>+(H25*H28*H27/365)</f>
-        <v>8.2082191780821923</v>
+        <v>150.41095890410958</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="20">
+      <c r="K31" s="19">
         <f>+(K25*K28*K27/365)</f>
-        <v>17.402739726027399</v>
+        <v>226.02739726027397</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="9"/>
+      <c r="B32" s="8"/>
       <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="19">
         <f>+B3*E9*E28/365</f>
-        <v>459.58904109589042</v>
+        <v>150.41095890410958</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="20">
+      <c r="H32" s="19">
         <f>+E41+E18+H30+H10</f>
-        <v>2861.3335616438353</v>
+        <v>225.75342465753425</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K32" s="19">
         <f>+E41+E18+H41+H18+K30+K10</f>
-        <v>4716.4842465753427</v>
+        <v>250.95890410958904</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
+      <c r="B33" s="8"/>
       <c r="D33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="19">
         <f>+IF(E31&gt;E32,+E32,+E31)</f>
-        <v>1.6712328767123288</v>
+        <v>75.205479452054789</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="20">
+      <c r="H33" s="19">
         <f>+IF(H31&gt;H32,+H32,+H31)</f>
-        <v>8.2082191780821923</v>
+        <v>150.41095890410958</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="20">
+      <c r="K33" s="19">
         <f>+IF(K31&gt;K32,+K32,+K31)</f>
-        <v>17.402739726027399</v>
+        <v>226.02739726027397</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="9"/>
-      <c r="E34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="K34" s="18"/>
+      <c r="B34" s="8"/>
+      <c r="E34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="9"/>
+      <c r="B35" s="8"/>
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K35" s="12">
+      <c r="K35" s="11">
         <f>$B$7</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="9"/>
+      <c r="B36" s="8"/>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="18">
         <f>+E30*E35</f>
-        <v>0.43660958904109587</v>
+        <v>10.027397260273974</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H36" s="18">
         <f>+H30*H35</f>
-        <v>0.32794520547945205</v>
+        <v>7.4794520547945211</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="19">
+      <c r="K36" s="18">
         <f>+K30*K35</f>
-        <v>0.48410958904109591</v>
+        <v>5.0410958904109595</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="9"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="9"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="9"/>
-      <c r="D39" s="13" t="s">
+      <c r="B39" s="8"/>
+      <c r="D39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="14"/>
-      <c r="G39" s="13" t="s">
+      <c r="E39" s="13"/>
+      <c r="G39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H39" s="14"/>
-      <c r="J39" s="13" t="s">
+      <c r="H39" s="13"/>
+      <c r="J39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K39" s="14"/>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="9"/>
-      <c r="D40" s="15" t="s">
+      <c r="B40" s="8"/>
+      <c r="D40" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="20">
         <f>+E25</f>
-        <v>500</v>
-      </c>
-      <c r="G40" s="15" t="s">
+        <v>5000</v>
+      </c>
+      <c r="G40" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="21">
+      <c r="H40" s="20">
         <f>+H25</f>
-        <v>700</v>
-      </c>
-      <c r="J40" s="15" t="s">
+        <v>5000</v>
+      </c>
+      <c r="J40" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K40" s="21">
+      <c r="K40" s="20">
         <f>+K25</f>
-        <v>800</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="9"/>
-      <c r="D41" s="15" t="s">
+      <c r="B41" s="8"/>
+      <c r="D41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="21">
+      <c r="E41" s="20">
         <f>+E30</f>
-        <v>2.297945205479452</v>
-      </c>
-      <c r="G41" s="15" t="s">
+        <v>50.136986301369866</v>
+      </c>
+      <c r="G41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="21">
+      <c r="H41" s="20">
         <f>+H30</f>
-        <v>1.726027397260274</v>
-      </c>
-      <c r="J41" s="15" t="s">
+        <v>37.397260273972606</v>
+      </c>
+      <c r="J41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="21">
+      <c r="K41" s="20">
         <f>+K30</f>
-        <v>2.547945205479452</v>
+        <v>25.205479452054796</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="9"/>
-      <c r="D42" s="15" t="s">
+      <c r="B42" s="8"/>
+      <c r="D42" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="20">
         <f>-E36</f>
-        <v>-0.43660958904109587</v>
-      </c>
-      <c r="G42" s="15" t="s">
+        <v>-10.027397260273974</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="21">
+      <c r="H42" s="20">
         <f>-H36</f>
-        <v>-0.32794520547945205</v>
-      </c>
-      <c r="J42" s="15" t="s">
+        <v>-7.4794520547945211</v>
+      </c>
+      <c r="J42" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K42" s="21">
+      <c r="K42" s="20">
         <f>-K36</f>
-        <v>-0.48410958904109591</v>
+        <v>-5.0410958904109595</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="9"/>
-      <c r="D43" s="15" t="s">
+      <c r="B43" s="8"/>
+      <c r="D43" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="21">
+      <c r="E43" s="20">
         <f>-E33</f>
-        <v>-1.6712328767123288</v>
-      </c>
-      <c r="G43" s="15" t="s">
+        <v>-75.205479452054789</v>
+      </c>
+      <c r="G43" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="21">
+      <c r="H43" s="20">
         <f>-H33</f>
-        <v>-8.2082191780821923</v>
-      </c>
-      <c r="J43" s="15" t="s">
+        <v>-150.41095890410958</v>
+      </c>
+      <c r="J43" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K43" s="21">
+      <c r="K43" s="20">
         <f>-K33</f>
-        <v>-17.402739726027399</v>
+        <v>-226.02739726027397</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D44" s="17"/>
-      <c r="E44" s="22">
+      <c r="D44" s="16"/>
+      <c r="E44" s="21">
         <f>+SUM(E40:E43)</f>
-        <v>500.190102739726</v>
-      </c>
-      <c r="G44" s="17"/>
-      <c r="H44" s="22">
+        <v>4964.9041095890416</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="21">
         <f>+SUM(H40:H43)</f>
-        <v>693.18986301369864</v>
-      </c>
-      <c r="J44" s="17"/>
-      <c r="K44" s="22">
+        <v>4879.5068493150675</v>
+      </c>
+      <c r="J44" s="16"/>
+      <c r="K44" s="21">
         <f>+SUM(K40:K43)</f>
-        <v>784.66109589041093</v>
+        <v>4794.1369863013697</v>
       </c>
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
@@ -1508,4 +1676,858 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="43"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="44"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="28">
+        <v>99999</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="28">
+        <v>99998</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="29">
+        <v>45265</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="29">
+        <v>45448</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="29">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="26">
+        <v>183</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="26">
+        <v>183</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="26">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="26">
+        <v>1</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="26">
+        <v>501.36</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="26">
+        <v>501.36</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="26">
+        <v>19</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="26">
+        <v>19</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="28">
+        <v>9525.93</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="28">
+        <v>9525.84</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="33">
+        <v>501.36</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="33">
+        <v>501.36</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="35">
+        <v>-9525.93</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="35">
+        <v>-9525.84</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="38">
+        <v>9024.57</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="38">
+        <v>9024.48</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="43"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="26">
+        <v>1</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="26">
+        <v>1</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="28">
+        <v>99998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="29">
+        <v>45264</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="29">
+        <v>45448</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="29">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="26">
+        <v>200</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="26">
+        <v>200</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="26">
+        <v>182</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="26">
+        <v>366</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="26">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="26">
+        <v>182</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="26">
+        <v>183</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="26">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="26">
+        <v>0</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="26">
+        <v>501.36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="26">
+        <v>1</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="26">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="28">
+        <v>300815.90000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="26">
+        <v>498.63</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="28">
+        <v>1002.73</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="28">
+        <v>1504.09</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="26">
+        <v>1</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="26">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="28">
+        <v>1504.09</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
+    </row>
+    <row r="35" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="26">
+        <v>19</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="26">
+        <v>19</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="26">
+        <v>0</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="26">
+        <v>0</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="26">
+        <v>95.26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="26"/>
+    </row>
+    <row r="38" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="26"/>
+    </row>
+    <row r="39" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="31"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="31"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="33">
+        <v>1</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="33">
+        <v>1</v>
+      </c>
+      <c r="F40" s="27"/>
+      <c r="G40" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="35">
+        <v>99998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="33">
+        <v>0</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="33">
+        <v>501.36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="33">
+        <v>0</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="27"/>
+      <c r="G42" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42" s="33">
+        <v>-95.26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="33">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="33">
+        <v>-2.0099999999999998</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="35">
+        <v>-1504.09</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37"/>
+      <c r="B44" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="39">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="27"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38">
+        <v>98900.01</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="25"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="25"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="26"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="26"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:H24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>